<commit_message>
fixed addUser and mostly fixed upload user.
changed the html in add user so you have a dropdown of companies/roles.
Fixed and tested the addUser. Also fixed but did not test the
uploadUser, it should work to upload. I have not added a way to add
roles or companies manually other than hard coding so the roles in the
excel sheet will have no permissions at all since their roles dont
really mean anything.
</commit_message>
<xml_diff>
--- a/WebBasedEvaluations/Documents/Review_Data_Upload_Users.xlsx
+++ b/WebBasedEvaluations/Documents/Review_Data_Upload_Users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalto\git\Master\Spring-2022---Web-Evaluation\WebBasedEvaluations\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\Fall-2022-Group-3-Web-Evaluation\WebBasedEvaluations\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA28EAF1-C89E-45A8-9827-B6AE47EA570A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BF92A8-5312-4214-B8F2-4ADB7E18B472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="0" windowWidth="21600" windowHeight="11332" xr2:uid="{22937C1E-74A3-40E4-BA81-B6A9358BF137}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22937C1E-74A3-40E4-BA81-B6A9358BF137}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="180">
   <si>
     <t>EMAIL</t>
   </si>
@@ -482,9 +485,6 @@
     <t>JOB TITLE</t>
   </si>
   <si>
-    <t>SUPERVISOR</t>
-  </si>
-  <si>
     <t>COMPANY NAME</t>
   </si>
   <si>
@@ -539,54 +539,9 @@
     <t>Quality Assurance</t>
   </si>
   <si>
-    <t>MARK HECKATHORNE</t>
-  </si>
-  <si>
-    <t>JEFFERY CHROSTOWSKI</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>MICHAEL CARNAHAN</t>
-  </si>
-  <si>
-    <t>SCOTT CALLAWAY</t>
-  </si>
-  <si>
-    <t>JOHN SCALO</t>
-  </si>
-  <si>
-    <t>LISA ELLEK</t>
-  </si>
-  <si>
-    <t>DEREK DENNICK</t>
-  </si>
-  <si>
-    <t>BRIAN EXLINE</t>
-  </si>
-  <si>
-    <t>MARY CRIVARO</t>
-  </si>
-  <si>
-    <t>PATRICIA CORREA</t>
-  </si>
-  <si>
-    <t>RYAN WACHTER</t>
-  </si>
-  <si>
-    <t>DONNA BODNAR</t>
-  </si>
-  <si>
-    <t>KEVIN HUFF</t>
-  </si>
-  <si>
-    <t>DAVE LANCASTER</t>
-  </si>
-  <si>
-    <t>JAY RADAKER</t>
-  </si>
-  <si>
     <t>Thangiah Manufacturing LLC</t>
   </si>
   <si>
@@ -594,6 +549,33 @@
   </si>
   <si>
     <t>EVALUATOR_EVAL</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Saftey</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>DEPT</t>
+  </si>
+  <si>
+    <t>Floor Crew</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Upper Management</t>
+  </si>
+  <si>
+    <t>DEPT MANAGER</t>
   </si>
 </sst>
 </file>
@@ -986,29 +968,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CD84BE-ACB0-4278-92AE-092DB62074A3}">
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.53125" customWidth="1"/>
-    <col min="3" max="3" width="8.86328125" customWidth="1"/>
-    <col min="4" max="4" width="33.86328125" customWidth="1"/>
-    <col min="5" max="5" width="74.86328125" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.86328125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
+    <col min="5" max="5" width="74.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="10" width="31" customWidth="1"/>
-    <col min="11" max="11" width="36.33203125" customWidth="1"/>
-    <col min="12" max="12" width="24.6640625" customWidth="1"/>
+    <col min="10" max="11" width="31" customWidth="1"/>
+    <col min="12" max="12" width="36.28515625" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -1016,7 +998,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1039,22 +1021,25 @@
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>148</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M2" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1069,7 +1054,7 @@
         <v>133</v>
       </c>
       <c r="F3" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -1078,19 +1063,22 @@
         <v>43831</v>
       </c>
       <c r="I3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K3" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="L3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1114,19 +1102,22 @@
         <v>43832</v>
       </c>
       <c r="I4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K4" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="L4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1141,7 +1132,7 @@
         <v>133</v>
       </c>
       <c r="F5" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -1150,19 +1141,22 @@
         <v>43833</v>
       </c>
       <c r="I5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J5" t="s">
-        <v>169</v>
-      </c>
-      <c r="K5" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1186,19 +1180,22 @@
         <v>43834</v>
       </c>
       <c r="I6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
-      </c>
-      <c r="K6" t="s">
-        <v>184</v>
+        <v>173</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1222,19 +1219,22 @@
         <v>43835</v>
       </c>
       <c r="I7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J7" t="s">
-        <v>168</v>
-      </c>
-      <c r="K7" t="s">
-        <v>184</v>
+        <v>173</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>133</v>
       </c>
       <c r="F8" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -1258,19 +1258,22 @@
         <v>43836</v>
       </c>
       <c r="I8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J8" t="s">
-        <v>169</v>
-      </c>
-      <c r="K8" t="s">
-        <v>184</v>
+        <v>173</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1294,19 +1297,22 @@
         <v>43837</v>
       </c>
       <c r="I9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J9" t="s">
-        <v>171</v>
-      </c>
-      <c r="K9" t="s">
-        <v>184</v>
+        <v>174</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -1330,19 +1336,22 @@
         <v>43838</v>
       </c>
       <c r="I10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J10" t="s">
-        <v>171</v>
-      </c>
-      <c r="K10" t="s">
-        <v>184</v>
+        <v>174</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1357,7 +1366,7 @@
         <v>133</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -1366,19 +1375,22 @@
         <v>43839</v>
       </c>
       <c r="I11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J11" t="s">
-        <v>169</v>
-      </c>
-      <c r="K11" t="s">
-        <v>184</v>
+        <v>174</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1402,19 +1414,22 @@
         <v>43840</v>
       </c>
       <c r="I12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J12" t="s">
-        <v>172</v>
-      </c>
-      <c r="K12" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1438,19 +1453,22 @@
         <v>43841</v>
       </c>
       <c r="I13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J13" t="s">
-        <v>172</v>
-      </c>
-      <c r="K13" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1474,19 +1492,22 @@
         <v>43842</v>
       </c>
       <c r="I14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J14" t="s">
-        <v>172</v>
-      </c>
-      <c r="K14" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1510,19 +1531,22 @@
         <v>43843</v>
       </c>
       <c r="I15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J15" t="s">
-        <v>172</v>
-      </c>
-      <c r="K15" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1546,19 +1570,22 @@
         <v>43844</v>
       </c>
       <c r="I16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K16" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1582,19 +1609,22 @@
         <v>43845</v>
       </c>
       <c r="I17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J17" t="s">
-        <v>172</v>
-      </c>
-      <c r="K17" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1612,7 +1642,7 @@
         <v>133</v>
       </c>
       <c r="F18" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -1621,19 +1651,22 @@
         <v>43846</v>
       </c>
       <c r="I18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J18" t="s">
-        <v>169</v>
-      </c>
-      <c r="K18" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1657,19 +1690,22 @@
         <v>43847</v>
       </c>
       <c r="I19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J19" t="s">
-        <v>173</v>
-      </c>
-      <c r="K19" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1684,7 +1720,7 @@
         <v>133</v>
       </c>
       <c r="F20" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -1693,19 +1729,22 @@
         <v>43848</v>
       </c>
       <c r="I20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J20" t="s">
-        <v>169</v>
-      </c>
-      <c r="K20" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1729,19 +1768,22 @@
         <v>43849</v>
       </c>
       <c r="I21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J21" t="s">
-        <v>174</v>
-      </c>
-      <c r="K21" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1765,19 +1807,22 @@
         <v>43850</v>
       </c>
       <c r="I22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J22" t="s">
-        <v>174</v>
-      </c>
-      <c r="K22" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1801,19 +1846,22 @@
         <v>43851</v>
       </c>
       <c r="I23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J23" t="s">
-        <v>174</v>
-      </c>
-      <c r="K23" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1837,19 +1885,22 @@
         <v>43852</v>
       </c>
       <c r="I24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J24" t="s">
-        <v>174</v>
-      </c>
-      <c r="K24" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1873,19 +1924,22 @@
         <v>43853</v>
       </c>
       <c r="I25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J25" t="s">
-        <v>174</v>
-      </c>
-      <c r="K25" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K25" t="b">
+        <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1909,19 +1963,22 @@
         <v>43854</v>
       </c>
       <c r="I26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J26" t="s">
-        <v>174</v>
-      </c>
-      <c r="K26" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1945,19 +2002,22 @@
         <v>43855</v>
       </c>
       <c r="I27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J27" t="s">
-        <v>174</v>
-      </c>
-      <c r="K27" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K27" t="b">
+        <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M27" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1981,19 +2041,22 @@
         <v>43856</v>
       </c>
       <c r="I28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J28" t="s">
-        <v>174</v>
-      </c>
-      <c r="K28" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K28" t="b">
+        <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -2017,19 +2080,22 @@
         <v>43857</v>
       </c>
       <c r="I29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J29" t="s">
-        <v>174</v>
-      </c>
-      <c r="K29" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K29" t="b">
+        <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2044,7 +2110,7 @@
         <v>133</v>
       </c>
       <c r="F30" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -2053,19 +2119,22 @@
         <v>43858</v>
       </c>
       <c r="I30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J30" t="s">
-        <v>169</v>
-      </c>
-      <c r="K30" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K30" t="b">
+        <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2080,7 +2149,7 @@
         <v>133</v>
       </c>
       <c r="F31" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
@@ -2089,19 +2158,22 @@
         <v>43859</v>
       </c>
       <c r="I31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J31" t="s">
-        <v>169</v>
-      </c>
-      <c r="K31" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K31" t="b">
+        <v>0</v>
       </c>
       <c r="L31" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -2125,19 +2197,22 @@
         <v>43860</v>
       </c>
       <c r="I32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J32" t="s">
-        <v>175</v>
-      </c>
-      <c r="K32" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K32" t="b">
+        <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2161,19 +2236,22 @@
         <v>43861</v>
       </c>
       <c r="I33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J33" t="s">
-        <v>175</v>
-      </c>
-      <c r="K33" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K33" t="b">
+        <v>0</v>
       </c>
       <c r="L33" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2197,19 +2275,22 @@
         <v>43862</v>
       </c>
       <c r="I34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J34" t="s">
-        <v>175</v>
-      </c>
-      <c r="K34" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K34" t="b">
+        <v>0</v>
       </c>
       <c r="L34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M34" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2224,7 +2305,7 @@
         <v>133</v>
       </c>
       <c r="F35" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G35" t="b">
         <v>1</v>
@@ -2233,19 +2314,22 @@
         <v>43863</v>
       </c>
       <c r="I35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J35" t="s">
-        <v>169</v>
-      </c>
-      <c r="K35" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K35" t="b">
+        <v>0</v>
       </c>
       <c r="L35" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -2260,7 +2344,7 @@
         <v>133</v>
       </c>
       <c r="F36" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -2269,19 +2353,22 @@
         <v>43864</v>
       </c>
       <c r="I36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J36" t="s">
-        <v>169</v>
-      </c>
-      <c r="K36" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K36" t="b">
+        <v>0</v>
       </c>
       <c r="L36" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>131</v>
       </c>
@@ -2308,19 +2395,22 @@
         <v>43865</v>
       </c>
       <c r="I37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J37" t="s">
-        <v>177</v>
-      </c>
-      <c r="K37" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K37" t="b">
+        <v>0</v>
       </c>
       <c r="L37" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -2344,19 +2434,22 @@
         <v>43866</v>
       </c>
       <c r="I38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J38" t="s">
-        <v>177</v>
-      </c>
-      <c r="K38" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K38" t="b">
+        <v>0</v>
       </c>
       <c r="L38" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2380,19 +2473,22 @@
         <v>43867</v>
       </c>
       <c r="I39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J39" t="s">
-        <v>177</v>
-      </c>
-      <c r="K39" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K39" t="b">
+        <v>0</v>
       </c>
       <c r="L39" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M39" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2416,19 +2512,22 @@
         <v>43868</v>
       </c>
       <c r="I40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J40" t="s">
-        <v>177</v>
-      </c>
-      <c r="K40" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K40" t="b">
+        <v>0</v>
       </c>
       <c r="L40" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -2452,19 +2551,22 @@
         <v>43869</v>
       </c>
       <c r="I41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J41" t="s">
-        <v>177</v>
-      </c>
-      <c r="K41" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K41" t="b">
+        <v>0</v>
       </c>
       <c r="L41" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M41" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -2488,19 +2590,22 @@
         <v>43870</v>
       </c>
       <c r="I42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J42" t="s">
-        <v>177</v>
-      </c>
-      <c r="K42" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K42" t="b">
+        <v>0</v>
       </c>
       <c r="L42" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M42" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -2524,19 +2629,22 @@
         <v>43871</v>
       </c>
       <c r="I43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J43" t="s">
-        <v>177</v>
-      </c>
-      <c r="K43" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K43" t="b">
+        <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -2560,19 +2668,22 @@
         <v>43872</v>
       </c>
       <c r="I44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J44" t="s">
-        <v>177</v>
-      </c>
-      <c r="K44" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K44" t="b">
+        <v>0</v>
       </c>
       <c r="L44" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -2596,19 +2707,22 @@
         <v>43873</v>
       </c>
       <c r="I45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J45" t="s">
-        <v>177</v>
-      </c>
-      <c r="K45" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="K45" t="b">
+        <v>0</v>
       </c>
       <c r="L45" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -2623,7 +2737,7 @@
         <v>133</v>
       </c>
       <c r="F46" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
@@ -2632,19 +2746,22 @@
         <v>43874</v>
       </c>
       <c r="I46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J46" t="s">
-        <v>169</v>
-      </c>
-      <c r="K46" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="K46" t="b">
+        <v>1</v>
       </c>
       <c r="L46" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M46" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2668,19 +2785,22 @@
         <v>43875</v>
       </c>
       <c r="I47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J47" t="s">
-        <v>178</v>
-      </c>
-      <c r="K47" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="K47" t="b">
+        <v>0</v>
       </c>
       <c r="L47" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M47" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2704,19 +2824,22 @@
         <v>43876</v>
       </c>
       <c r="I48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J48" t="s">
-        <v>178</v>
-      </c>
-      <c r="K48" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="K48" t="b">
+        <v>0</v>
       </c>
       <c r="L48" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M48" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2740,19 +2863,22 @@
         <v>43877</v>
       </c>
       <c r="I49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J49" t="s">
-        <v>178</v>
-      </c>
-      <c r="K49" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="K49" t="b">
+        <v>0</v>
       </c>
       <c r="L49" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -2776,19 +2902,22 @@
         <v>43878</v>
       </c>
       <c r="I50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J50" t="s">
-        <v>178</v>
-      </c>
-      <c r="K50" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="K50" t="b">
+        <v>0</v>
       </c>
       <c r="L50" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -2812,19 +2941,22 @@
         <v>43879</v>
       </c>
       <c r="I51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J51" t="s">
-        <v>178</v>
-      </c>
-      <c r="K51" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="K51" t="b">
+        <v>0</v>
       </c>
       <c r="L51" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -2839,7 +2971,7 @@
         <v>133</v>
       </c>
       <c r="F52" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G52" t="b">
         <v>1</v>
@@ -2848,19 +2980,22 @@
         <v>43880</v>
       </c>
       <c r="I52" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J52" t="s">
-        <v>169</v>
-      </c>
-      <c r="K52" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K52" t="b">
+        <v>1</v>
       </c>
       <c r="L52" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -2884,19 +3019,22 @@
         <v>43881</v>
       </c>
       <c r="I53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J53" t="s">
-        <v>179</v>
-      </c>
-      <c r="K53" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K53" t="b">
+        <v>0</v>
       </c>
       <c r="L53" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M53" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>30</v>
       </c>
@@ -2920,19 +3058,22 @@
         <v>43882</v>
       </c>
       <c r="I54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J54" t="s">
-        <v>179</v>
-      </c>
-      <c r="K54" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K54" t="b">
+        <v>0</v>
       </c>
       <c r="L54" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M54" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -2956,19 +3097,22 @@
         <v>43883</v>
       </c>
       <c r="I55" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J55" t="s">
-        <v>179</v>
-      </c>
-      <c r="K55" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K55" t="b">
+        <v>0</v>
       </c>
       <c r="L55" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2992,19 +3136,22 @@
         <v>43884</v>
       </c>
       <c r="I56" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J56" t="s">
-        <v>179</v>
-      </c>
-      <c r="K56" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K56" t="b">
+        <v>0</v>
       </c>
       <c r="L56" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M56" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -3028,19 +3175,22 @@
         <v>43885</v>
       </c>
       <c r="I57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J57" t="s">
-        <v>179</v>
-      </c>
-      <c r="K57" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K57" t="b">
+        <v>0</v>
       </c>
       <c r="L57" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M57" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -3064,19 +3214,22 @@
         <v>43886</v>
       </c>
       <c r="I58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J58" t="s">
-        <v>179</v>
-      </c>
-      <c r="K58" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K58" t="b">
+        <v>0</v>
       </c>
       <c r="L58" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M58" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -3100,19 +3253,22 @@
         <v>43887</v>
       </c>
       <c r="I59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J59" t="s">
-        <v>179</v>
-      </c>
-      <c r="K59" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K59" t="b">
+        <v>0</v>
       </c>
       <c r="L59" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M59" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -3136,19 +3292,22 @@
         <v>43888</v>
       </c>
       <c r="I60" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J60" t="s">
-        <v>179</v>
-      </c>
-      <c r="K60" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K60" t="b">
+        <v>0</v>
       </c>
       <c r="L60" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M60" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -3172,19 +3331,22 @@
         <v>43889</v>
       </c>
       <c r="I61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J61" t="s">
-        <v>179</v>
-      </c>
-      <c r="K61" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K61" t="b">
+        <v>0</v>
       </c>
       <c r="L61" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M61" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -3208,19 +3370,22 @@
         <v>43890</v>
       </c>
       <c r="I62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J62" t="s">
-        <v>179</v>
-      </c>
-      <c r="K62" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K62" t="b">
+        <v>0</v>
       </c>
       <c r="L62" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M62" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -3244,19 +3409,22 @@
         <v>43891</v>
       </c>
       <c r="I63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J63" t="s">
-        <v>179</v>
-      </c>
-      <c r="K63" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K63" t="b">
+        <v>0</v>
       </c>
       <c r="L63" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M63" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -3280,19 +3448,22 @@
         <v>43892</v>
       </c>
       <c r="I64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J64" t="s">
-        <v>179</v>
-      </c>
-      <c r="K64" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K64" t="b">
+        <v>0</v>
       </c>
       <c r="L64" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M64" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -3316,19 +3487,22 @@
         <v>43893</v>
       </c>
       <c r="I65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J65" t="s">
-        <v>179</v>
-      </c>
-      <c r="K65" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K65" t="b">
+        <v>0</v>
       </c>
       <c r="L65" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M65" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>145</v>
       </c>
@@ -3352,19 +3526,22 @@
         <v>43894</v>
       </c>
       <c r="I66" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J66" t="s">
-        <v>179</v>
-      </c>
-      <c r="K66" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="K66" t="b">
+        <v>0</v>
       </c>
       <c r="L66" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M66" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -3379,7 +3556,7 @@
         <v>133</v>
       </c>
       <c r="F67" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G67" t="b">
         <v>1</v>
@@ -3388,19 +3565,22 @@
         <v>43895</v>
       </c>
       <c r="I67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J67" t="s">
-        <v>169</v>
-      </c>
-      <c r="K67" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K67" t="b">
+        <v>1</v>
       </c>
       <c r="L67" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M67" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -3415,7 +3595,7 @@
         <v>133</v>
       </c>
       <c r="F68" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G68" t="b">
         <v>1</v>
@@ -3424,19 +3604,22 @@
         <v>43896</v>
       </c>
       <c r="I68" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J68" t="s">
-        <v>180</v>
-      </c>
-      <c r="K68" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K68" t="b">
+        <v>0</v>
       </c>
       <c r="L68" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M68" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>61</v>
       </c>
@@ -3451,7 +3634,7 @@
         <v>133</v>
       </c>
       <c r="F69" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G69" t="b">
         <v>1</v>
@@ -3460,19 +3643,22 @@
         <v>43897</v>
       </c>
       <c r="I69" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J69" t="s">
-        <v>169</v>
-      </c>
-      <c r="K69" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K69" t="b">
+        <v>0</v>
       </c>
       <c r="L69" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M69" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>58</v>
       </c>
@@ -3496,19 +3682,22 @@
         <v>43898</v>
       </c>
       <c r="I70" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J70" t="s">
-        <v>181</v>
-      </c>
-      <c r="K70" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K70" t="b">
+        <v>0</v>
       </c>
       <c r="L70" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M70" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>65</v>
       </c>
@@ -3523,7 +3712,7 @@
         <v>133</v>
       </c>
       <c r="F71" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G71" t="b">
         <v>1</v>
@@ -3532,19 +3721,22 @@
         <v>43899</v>
       </c>
       <c r="I71" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J71" t="s">
-        <v>169</v>
-      </c>
-      <c r="K71" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K71" t="b">
+        <v>0</v>
       </c>
       <c r="L71" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M71" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>66</v>
       </c>
@@ -3568,19 +3760,22 @@
         <v>43900</v>
       </c>
       <c r="I72" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J72" t="s">
-        <v>182</v>
-      </c>
-      <c r="K72" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K72" t="b">
+        <v>0</v>
       </c>
       <c r="L72" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M72" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -3595,7 +3790,7 @@
         <v>133</v>
       </c>
       <c r="F73" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G73" t="b">
         <v>1</v>
@@ -3604,19 +3799,22 @@
         <v>43901</v>
       </c>
       <c r="I73" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J73" t="s">
-        <v>169</v>
-      </c>
-      <c r="K73" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K73" t="b">
+        <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M73" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>68</v>
       </c>
@@ -3640,19 +3838,22 @@
         <v>43902</v>
       </c>
       <c r="I74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J74" t="s">
-        <v>183</v>
-      </c>
-      <c r="K74" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K74" t="b">
+        <v>0</v>
       </c>
       <c r="L74" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M74" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>69</v>
       </c>
@@ -3676,19 +3877,22 @@
         <v>43903</v>
       </c>
       <c r="I75" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J75" t="s">
-        <v>183</v>
-      </c>
-      <c r="K75" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K75" t="b">
+        <v>0</v>
       </c>
       <c r="L75" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M75" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>60</v>
       </c>
@@ -3712,19 +3916,22 @@
         <v>43904</v>
       </c>
       <c r="I76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J76" t="s">
-        <v>183</v>
-      </c>
-      <c r="K76" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K76" t="b">
+        <v>0</v>
       </c>
       <c r="L76" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M76" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -3748,19 +3955,22 @@
         <v>43905</v>
       </c>
       <c r="I77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J77" t="s">
-        <v>169</v>
-      </c>
-      <c r="K77" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K77" t="b">
+        <v>0</v>
       </c>
       <c r="L77" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M77" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>137</v>
       </c>
@@ -3784,19 +3994,22 @@
         <v>43906</v>
       </c>
       <c r="I78" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J78" t="s">
-        <v>169</v>
-      </c>
-      <c r="K78" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K78" t="b">
+        <v>0</v>
       </c>
       <c r="L78" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M78" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>138</v>
       </c>
@@ -3820,19 +4033,22 @@
         <v>43907</v>
       </c>
       <c r="I79" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J79" t="s">
-        <v>169</v>
-      </c>
-      <c r="K79" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K79" t="b">
+        <v>0</v>
       </c>
       <c r="L79" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M79" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>139</v>
       </c>
@@ -3856,19 +4072,22 @@
         <v>43908</v>
       </c>
       <c r="I80" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J80" t="s">
-        <v>169</v>
-      </c>
-      <c r="K80" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K80" t="b">
+        <v>0</v>
       </c>
       <c r="L80" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M80" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>140</v>
       </c>
@@ -3892,19 +4111,22 @@
         <v>43909</v>
       </c>
       <c r="I81" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J81" t="s">
-        <v>169</v>
-      </c>
-      <c r="K81" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K81" t="b">
+        <v>0</v>
       </c>
       <c r="L81" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M81" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>141</v>
       </c>
@@ -3928,19 +4150,22 @@
         <v>43910</v>
       </c>
       <c r="I82" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J82" t="s">
-        <v>169</v>
-      </c>
-      <c r="K82" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K82" t="b">
+        <v>0</v>
       </c>
       <c r="L82" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+      <c r="M82" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>138</v>
       </c>
@@ -3964,16 +4189,19 @@
         <v>43911</v>
       </c>
       <c r="I83" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J83" t="s">
-        <v>169</v>
-      </c>
-      <c r="K83" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="K83" t="b">
+        <v>0</v>
       </c>
       <c r="L83" t="s">
-        <v>185</v>
+        <v>168</v>
+      </c>
+      <c r="M83" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding excel files to commit
</commit_message>
<xml_diff>
--- a/WebBasedEvaluations/Documents/Review_Data_Upload_Users.xlsx
+++ b/WebBasedEvaluations/Documents/Review_Data_Upload_Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\Fall-2022-Group-3-Web-Evaluation\WebBasedEvaluations\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BF92A8-5312-4214-B8F2-4ADB7E18B472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD668D4-59BC-45CE-815B-7E6849FC0433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22937C1E-74A3-40E4-BA81-B6A9358BF137}"/>
   </bookViews>
@@ -970,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CD84BE-ACB0-4278-92AE-092DB62074A3}">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,7 +981,7 @@
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" customWidth="1"/>
     <col min="5" max="5" width="74.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>

</xml_diff>